<commit_message>
Updated Plots and Results File
</commit_message>
<xml_diff>
--- a/data/word2vec_Results.xlsx
+++ b/data/word2vec_Results.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vatsal\OneDrive\NLP_Project\DeepNews\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vatsal\OneDrive\NLP_Project\DeepNews\word2vec\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="23">
   <si>
     <t>Model</t>
   </si>
@@ -183,24 +184,17 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-IN"/>
-              <a:t>Word2Vec</a:t>
+              <a:t>Word2Vec Accuracy Improvement for Total Dataset</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-IN" baseline="0"/>
-              <a:t> Accuracy Improvement on Total Dataset vs Fire Dataset</a:t>
+              <a:t> vs Fire Dataset</a:t>
             </a:r>
             <a:endParaRPr lang="en-IN"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.18795774034221818"/>
-          <c:y val="2.3494912451012116E-2"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -232,17 +226,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="7.8218987566793172E-2"/>
-          <c:y val="0.13183561643835617"/>
-          <c:w val="0.9005326724597672"/>
-          <c:h val="0.48384683421421637"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -256,7 +240,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Best Match Correct</c:v>
+                  <c:v>Opposite Correct</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -380,7 +364,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Best Match Topk </c:v>
+                  <c:v>Opposite Topk </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -504,7 +488,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Opposite Correct</c:v>
+                  <c:v>Best Match Correct</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -628,7 +612,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Opposite Topk </c:v>
+                  <c:v>Best Match Topk </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -753,11 +737,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1788466704"/>
-        <c:axId val="1788468880"/>
+        <c:axId val="-1091871296"/>
+        <c:axId val="-1091870752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1788466704"/>
+        <c:axId val="-1091871296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -856,7 +840,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1788468880"/>
+        <c:crossAx val="-1091870752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -864,7 +848,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1788468880"/>
+        <c:axId val="-1091870752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -971,7 +955,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1788466704"/>
+        <c:crossAx val="-1091871296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -985,16 +969,837 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="8.5483052408568808E-2"/>
-          <c:y val="0.87126730086335891"/>
-          <c:w val="0.78840288285351445"/>
-          <c:h val="0.10523784225947756"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IN"/>
+              <a:t>Improvement in Word2Vec</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IN" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IN"/>
+              <a:t>Accuracy with</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IN" baseline="0"/>
+              <a:t> change in Window size and Negative </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IN"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:line3DChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Opposite Correct</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>100d_w5_n5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100d_w10_n25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100d_w15_n40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100d_w25_n50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100d_w5_n5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100d_w15_n40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100d_w10_n25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>300d_w5_n5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>300d_w5_n5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100d_w25_n50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>300d_w10_n25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>300d_w15_n40</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$2:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Opposite Topk </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>100d_w5_n5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100d_w10_n25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100d_w15_n40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100d_w25_n50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100d_w5_n5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100d_w15_n40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100d_w10_n25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>300d_w5_n5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>300d_w5_n5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100d_w25_n50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>300d_w10_n25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>300d_w15_n40</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$C$2:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Best Match Correct</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>100d_w5_n5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100d_w10_n25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100d_w15_n40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100d_w25_n50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100d_w5_n5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100d_w15_n40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100d_w10_n25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>300d_w5_n5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>300d_w5_n5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100d_w25_n50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>300d_w10_n25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>300d_w15_n40</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$D$2:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Best Match Topk </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>100d_w5_n5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100d_w10_n25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100d_w15_n40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100d_w25_n50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100d_w5_n5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100d_w15_n40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100d_w10_n25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>300d_w5_n5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>300d_w5_n5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100d_w25_n50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>300d_w10_n25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>300d_w15_n40</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$E$2:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28.3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>31.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-948452528"/>
+        <c:axId val="-948449808"/>
+        <c:axId val="-1091196688"/>
+      </c:line3DChart>
+      <c:catAx>
+        <c:axId val="-948452528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-948449808"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-948449808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-948452528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="-1091196688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-948449808"/>
+        <c:crosses val="autoZero"/>
+      </c:serAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1102,6 +1907,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1605,20 +2450,649 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="307">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>495299</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>142874</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.08498</cdr:x>
+      <cdr:y>0.11449</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.36438</cdr:x>
+      <cdr:y>0.21729</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="695326" y="466725"/>
+          <a:ext cx="2286000" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1400" b="1"/>
+            <a:t>Fire + Crawled</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IN" sz="1100" b="1"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.67986</cdr:x>
+      <cdr:y>0.11449</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.93481</cdr:x>
+      <cdr:y>0.25701</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5562601" y="466725"/>
+          <a:ext cx="2085975" cy="581025"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1400" b="1"/>
+            <a:t>Fire Dataset</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1019174</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>352424</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1640,16 +3114,16 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.03128</cdr:x>
-      <cdr:y>0.03377</cdr:y>
+      <cdr:x>0.06863</cdr:x>
+      <cdr:y>0.78442</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.18524</cdr:x>
-      <cdr:y>0.31571</cdr:y>
+      <cdr:x>0.36765</cdr:x>
+      <cdr:y>0.89312</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -1658,30 +3132,38 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="185738" y="109539"/>
-          <a:ext cx="914400" cy="914400"/>
+          <a:off x="533400" y="4124325"/>
+          <a:ext cx="2324100" cy="571500"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </cdr:spPr>
       <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:endParaRPr lang="en-IN" sz="1100"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1200" b="1" baseline="0"/>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1200" b="1"/>
+            <a:t>100 dimensional Word2Vec</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IN" sz="1100" b="1"/>
         </a:p>
       </cdr:txBody>
     </cdr:sp>
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.18043</cdr:x>
-      <cdr:y>0.11307</cdr:y>
+      <cdr:x>0.45833</cdr:x>
+      <cdr:y>0.83152</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.3344</cdr:x>
-      <cdr:y>0.39501</cdr:y>
+      <cdr:x>0.71324</cdr:x>
+      <cdr:y>0.9058</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -1690,87 +3172,20 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1071563" y="366713"/>
-          <a:ext cx="914400" cy="914400"/>
+          <a:off x="3562350" y="4371975"/>
+          <a:ext cx="1981200" cy="390525"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </cdr:spPr>
       <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-IN" sz="1400" b="1"/>
-            <a:t>Fire + Crawled</a:t>
-          </a:r>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.72253</cdr:x>
-      <cdr:y>0.11601</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.8765</cdr:x>
-      <cdr:y>0.39794</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="4" name="TextBox 3"/>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="4291013" y="376239"/>
-          <a:ext cx="914400" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:endParaRPr lang="en-IN" sz="1100"/>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.75942</cdr:x>
-      <cdr:y>0.11013</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.91339</cdr:x>
-      <cdr:y>0.39207</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="5" name="TextBox 4"/>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="4510088" y="357189"/>
-          <a:ext cx="914400" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-IN" sz="1400" b="1"/>
-            <a:t>Fire</a:t>
+            <a:rPr lang="en-IN" sz="1200" b="1"/>
+            <a:t>300 dimensional Word2Vec</a:t>
           </a:r>
           <a:endParaRPr lang="en-IN" sz="1100" b="1"/>
         </a:p>
@@ -2520,8 +3935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2539,16 +3954,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2796,4 +4211,251 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C2">
+        <v>8.6</v>
+      </c>
+      <c r="D2">
+        <v>3.1</v>
+      </c>
+      <c r="E2">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>2.8</v>
+      </c>
+      <c r="C3">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>3.4</v>
+      </c>
+      <c r="C4">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D4">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E4">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>2.9</v>
+      </c>
+      <c r="C5">
+        <v>7.7</v>
+      </c>
+      <c r="D5">
+        <v>4.7</v>
+      </c>
+      <c r="E5">
+        <v>17.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>3.1</v>
+      </c>
+      <c r="C6">
+        <v>10.1</v>
+      </c>
+      <c r="D6">
+        <v>8.6</v>
+      </c>
+      <c r="E6">
+        <v>19.600000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>3.7</v>
+      </c>
+      <c r="C7">
+        <v>9.6</v>
+      </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>23.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>3.6</v>
+      </c>
+      <c r="C8">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D8">
+        <v>10.4</v>
+      </c>
+      <c r="E8">
+        <v>24.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>3.7</v>
+      </c>
+      <c r="C10">
+        <v>12.1</v>
+      </c>
+      <c r="D10">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E10">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>4.5</v>
+      </c>
+      <c r="C11">
+        <v>14.5</v>
+      </c>
+      <c r="D11">
+        <v>9.9</v>
+      </c>
+      <c r="E11">
+        <v>24.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>3.3</v>
+      </c>
+      <c r="C12">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="D12">
+        <v>9.1</v>
+      </c>
+      <c r="E12">
+        <v>25.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C13">
+        <v>13.3</v>
+      </c>
+      <c r="D13">
+        <v>12.1</v>
+      </c>
+      <c r="E13">
+        <v>28.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>5.3</v>
+      </c>
+      <c r="C14">
+        <v>13.3</v>
+      </c>
+      <c r="D14">
+        <v>12.3</v>
+      </c>
+      <c r="E14">
+        <v>31.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:E13">
+    <sortCondition ref="E2:E13"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>